<commit_message>
finishes metadata excels and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/delta_entry_recapture_metadata.xlsx
+++ b/data-raw/metadata/delta_entry_recapture_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-lower-feather-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-delta-entry-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C43B39-D11A-0D4A-BBAD-89B2512FBBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA7F26C-5BE4-F840-9D3D-C5BC35DF58CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>whole</t>
   </si>
   <si>
-    <t>Whether the count (n) is an actual count or estimate. Levels = c("Yes", "No")</t>
-  </si>
-  <si>
     <t>visitTime</t>
   </si>
   <si>
@@ -205,55 +202,58 @@
     <t>recapture</t>
   </si>
   <si>
-    <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 12</t>
-  </si>
-  <si>
-    <t>Lower Feather River RST</t>
-  </si>
-  <si>
-    <t>Common name of species. Level = "Chinook salmon"</t>
-  </si>
-  <si>
-    <t>Run as assigned at the time of the capture. Levels = c("Not recorded", "Fall")</t>
-  </si>
-  <si>
-    <t>Run revised after field visit. Levels = c("Not recorded", "Fall")</t>
-  </si>
-  <si>
-    <t>Origin/production type of the fish. Levels = c("Natural", "Hatchery")</t>
-  </si>
-  <si>
-    <t>Life stage of the fish. Levels = c("Not recorded", "Parr")</t>
-  </si>
-  <si>
-    <t>Work that was done during visit to trap. Levels =c("Continue trapping", "Unplanned restart")</t>
-  </si>
-  <si>
-    <t>Name of the sampling site. Level  = "Lower Feather River RST"</t>
-  </si>
-  <si>
-    <t>Name of the trap or trap location. Levels = c("RL", "RR")</t>
-  </si>
-  <si>
-    <t>type of mark on fish. Level = "Pigment / dye"</t>
-  </si>
-  <si>
-    <t>color of mark on fish. Level = "Brown"</t>
-  </si>
-  <si>
-    <t>position of mark on body of fish. Level = "whole body"</t>
-  </si>
-  <si>
     <t>mort</t>
-  </si>
-  <si>
-    <t>Mortality. Levels = c("Yes", "No")</t>
   </si>
   <si>
     <t>actualCountID</t>
   </si>
   <si>
     <t>Number corresponding to actualCount value</t>
+  </si>
+  <si>
+    <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 10.</t>
+  </si>
+  <si>
+    <t>Delta Entry RST</t>
+  </si>
+  <si>
+    <t>Common name of species.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run as assigned at the time of the capture. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run revised after field visit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Origin/production type of the fish. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life stage of the fish. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortality. </t>
+  </si>
+  <si>
+    <t>Whether the count (n) is an actual count or estimate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work that was done during visit to trap. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the sampling site. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the trap or trap location. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">type of mark on fish. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">color of mark on fish. </t>
+  </si>
+  <si>
+    <t>position of mark on body of fish.</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -647,13 +647,13 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
@@ -691,7 +691,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>19</v>
@@ -729,7 +729,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>19</v>
@@ -761,13 +761,13 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -805,7 +805,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
@@ -834,16 +834,16 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
@@ -872,16 +872,16 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>19</v>
@@ -913,13 +913,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
@@ -951,13 +951,13 @@
         <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>19</v>
@@ -986,16 +986,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
@@ -1071,7 +1071,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>30</v>
@@ -1080,7 +1080,7 @@
         <v>29</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>31</v>
@@ -1119,7 +1119,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>30</v>
@@ -1128,7 +1128,7 @@
         <v>29</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>31</v>
@@ -1167,7 +1167,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>30</v>
@@ -1176,7 +1176,7 @@
         <v>29</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>36</v>
@@ -1185,10 +1185,10 @@
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
       <c r="L15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1206,16 +1206,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
@@ -1244,34 +1244,30 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="6"/>
       <c r="J17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K17" s="6"/>
-      <c r="L17" s="11">
-        <v>44594.41678240741</v>
-      </c>
-      <c r="M17" s="11">
-        <v>44679.479571759257</v>
-      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -1288,16 +1284,16 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>19</v>
@@ -1326,16 +1322,16 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
@@ -1364,16 +1360,16 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
@@ -1402,16 +1398,16 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>19</v>
@@ -1440,16 +1436,16 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>19</v>
@@ -1478,16 +1474,16 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>19</v>
@@ -1516,16 +1512,16 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>19</v>
@@ -28586,13 +28582,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28620,10 +28616,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>

</xml_diff>